<commit_message>
Built site for kwb.umberto: 0.2.0@31d51de
</commit_message>
<xml_diff>
--- a/reference/umberto10_results.xlsx
+++ b/reference/umberto10_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -31,64 +31,64 @@
     <t xml:space="preserve">0_Reference_Agri</t>
   </si>
   <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - climate change w/o LT, GWP100 w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T03: Activated  sludge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T06: CHP plant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T07: Centrifuge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T10: Effluent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T14: Polymer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T15: Sludge transport [RER]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T21: fertilizer substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T31: Electricity credits [ES]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T4: Electricity [IL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - freshwater ecotoxicity w/o LT, FETPinf w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - freshwater eutrophication w/o LT, FEP w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - human toxicity w/o LT, HTPinf w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - marine ecotoxicity w/o LT, METPinf w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - marine eutrophication w/o LT, MEP w/o LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - terrestrial acidification w/o LT, TAP100 w/o LT</t>
+  </si>
+  <si>
     <t xml:space="preserve">cumulative energy demand - fossil, non-renewable energy resources, fossil</t>
   </si>
   <si>
-    <t xml:space="preserve">T03: Activated  sludge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T06: CHP plant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T07: Centrifuge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T10: Effluent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T14: Polymer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T15: Sludge transport [RER]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T21: fertilizer substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T31: Electricity credits [ES]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T4: Electricity [IL]</t>
-  </si>
-  <si>
     <t xml:space="preserve">cumulative energy demand - nuclear, non-renewable energy resources, nuclear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - climate change w/o LT, GWP100 w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - freshwater ecotoxicity w/o LT, FETPinf w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - freshwater eutrophication w/o LT, FEP w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - human toxicity w/o LT, HTPinf w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - marine ecotoxicity w/o LT, METPinf w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - marine eutrophication w/o LT, MEP w/o LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - terrestrial acidification w/o LT, TAP100 w/o LT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -407,12 +407,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -432,7 +432,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="n">
+        <v>3780859.08311696</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -441,7 +443,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" t="n">
+        <v>180611.722614507</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -450,7 +454,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4"/>
+      <c r="C4" t="n">
+        <v>289428.775432367</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -469,7 +475,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>10433116.9438371</v>
+        <v>392609.350571056</v>
       </c>
     </row>
     <row r="7">
@@ -480,7 +486,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>1762.82923822559</v>
+        <v>110.077708792406</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +497,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-7072323.08092806</v>
+        <v>-217231.523240712</v>
       </c>
     </row>
     <row r="9">
@@ -502,7 +508,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-13154124.1204715</v>
+        <v>-1172632.84519849</v>
       </c>
     </row>
     <row r="10">
@@ -513,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>181431756.306697</v>
+        <v>13314949.1388226</v>
       </c>
     </row>
   </sheetData>
@@ -523,12 +529,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -585,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>296075.355505227</v>
+        <v>281.204698933857</v>
       </c>
     </row>
     <row r="7">
@@ -596,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>38.8605254313039</v>
+        <v>0.0843318098494594</v>
       </c>
     </row>
     <row r="8">
@@ -607,7 +613,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-712713.211781755</v>
+        <v>-2759.6585950617</v>
       </c>
     </row>
     <row r="9">
@@ -618,7 +624,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-12325698.9368461</v>
+        <v>-308.271724439994</v>
       </c>
     </row>
     <row r="10">
@@ -629,7 +635,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>542344.893745249</v>
+        <v>2056.05362640351</v>
       </c>
     </row>
   </sheetData>
@@ -639,12 +645,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -664,9 +670,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>3780859.08311696</v>
-      </c>
+      <c r="C2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -675,9 +679,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>180611.722614507</v>
-      </c>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -686,9 +688,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="n">
-        <v>289428.775432367</v>
-      </c>
+      <c r="C4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -697,7 +697,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="n">
+        <v>3009.67715207925</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -707,7 +709,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>392609.350571056</v>
+        <v>8.99061191069666</v>
       </c>
     </row>
     <row r="7">
@@ -718,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>110.077708792406</v>
+        <v>0.00160311891525617</v>
       </c>
     </row>
     <row r="8">
@@ -729,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-217231.523240712</v>
+        <v>1860.96549371055</v>
       </c>
     </row>
     <row r="9">
@@ -740,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-1172632.84519849</v>
+        <v>-54.0808142552251</v>
       </c>
     </row>
     <row r="10">
@@ -751,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>13314949.1388226</v>
+        <v>770.450190589926</v>
       </c>
     </row>
   </sheetData>
@@ -761,12 +763,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -823,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>281.204698933857</v>
+        <v>23784.5824592949</v>
       </c>
     </row>
     <row r="7">
@@ -834,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0843318098494595</v>
+        <v>23.22929811789</v>
       </c>
     </row>
     <row r="8">
@@ -845,7 +847,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-2759.6585950617</v>
+        <v>-110027.964095341</v>
       </c>
     </row>
     <row r="9">
@@ -856,7 +858,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-308.271724439994</v>
+        <v>-75226.2696774404</v>
       </c>
     </row>
     <row r="10">
@@ -867,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>2056.05362640351</v>
+        <v>571686.709419825</v>
       </c>
     </row>
   </sheetData>
@@ -877,12 +879,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -929,9 +931,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
-        <v>3009.67715207925</v>
-      </c>
+      <c r="C5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -941,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>8.99061191069666</v>
+        <v>384.798405223609</v>
       </c>
     </row>
     <row r="7">
@@ -952,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00160311891525617</v>
+        <v>0.391233296339834</v>
       </c>
     </row>
     <row r="8">
@@ -963,7 +963,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>1860.96549371055</v>
+        <v>-1821.71691243872</v>
       </c>
     </row>
     <row r="9">
@@ -974,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-54.0808142552251</v>
+        <v>-548.779480037789</v>
       </c>
     </row>
     <row r="10">
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>770.450190589926</v>
+        <v>3172.68059006507</v>
       </c>
     </row>
   </sheetData>
@@ -995,12 +995,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1020,7 +1020,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="n">
+        <v>592.173807043028</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1029,7 +1031,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" t="n">
+        <v>96.6791887850331</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1047,7 +1051,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="n">
+        <v>261651.314309439</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -1057,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>23784.5824592949</v>
+        <v>1437.33152509733</v>
       </c>
     </row>
     <row r="7">
@@ -1068,7 +1074,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>23.22929811789</v>
+        <v>0.0139564028473857</v>
       </c>
     </row>
     <row r="8">
@@ -1079,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-110027.964095341</v>
+        <v>10612.5042510072</v>
       </c>
     </row>
     <row r="9">
@@ -1090,7 +1096,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-75226.2696774404</v>
+        <v>-171.380370107561</v>
       </c>
     </row>
     <row r="10">
@@ -1101,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>571686.709419825</v>
+        <v>1393.38228094482</v>
       </c>
     </row>
   </sheetData>
@@ -1111,12 +1117,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1136,7 +1142,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="n">
+        <v>15769.8459484285</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1145,7 +1153,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3"/>
+      <c r="C3" t="n">
+        <v>9115.62157131185</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1173,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>384.798405223609</v>
+        <v>2142.13681635859</v>
       </c>
     </row>
     <row r="7">
@@ -1184,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.391233296339834</v>
+        <v>0.34340773994572</v>
       </c>
     </row>
     <row r="8">
@@ -1195,7 +1205,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-1821.71691243872</v>
+        <v>33056.0200547611</v>
       </c>
     </row>
     <row r="9">
@@ -1206,7 +1216,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-548.779480037789</v>
+        <v>-8259.3853040454</v>
       </c>
     </row>
     <row r="10">
@@ -1217,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>3172.68059006507</v>
+        <v>74116.3582598173</v>
       </c>
     </row>
   </sheetData>
@@ -1227,12 +1237,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1252,9 +1262,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>592.173807043028</v>
-      </c>
+      <c r="C2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1263,9 +1271,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>96.6791887850331</v>
-      </c>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1283,9 +1289,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
-        <v>261651.314309439</v>
-      </c>
+      <c r="C5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -1295,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1437.33152509733</v>
+        <v>10433116.9438371</v>
       </c>
     </row>
     <row r="7">
@@ -1306,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0139564028473857</v>
+        <v>1762.82923822559</v>
       </c>
     </row>
     <row r="8">
@@ -1317,7 +1321,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>10612.5042510072</v>
+        <v>-7072323.08092806</v>
       </c>
     </row>
     <row r="9">
@@ -1328,7 +1332,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-171.380370107561</v>
+        <v>-13154124.1204715</v>
       </c>
     </row>
     <row r="10">
@@ -1339,7 +1343,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>1393.38228094482</v>
+        <v>181431756.306697</v>
       </c>
     </row>
   </sheetData>
@@ -1349,12 +1353,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1374,9 +1378,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>15769.8459484285</v>
-      </c>
+      <c r="C2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1385,9 +1387,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>9115.62157131185</v>
-      </c>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -1415,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>2142.13681635859</v>
+        <v>296075.355505227</v>
       </c>
     </row>
     <row r="7">
@@ -1426,7 +1426,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.34340773994572</v>
+        <v>38.8605254313039</v>
       </c>
     </row>
     <row r="8">
@@ -1437,7 +1437,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>33056.0200547611</v>
+        <v>-712713.211781755</v>
       </c>
     </row>
     <row r="9">
@@ -1448,7 +1448,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-8259.3853040454</v>
+        <v>-12325698.9368461</v>
       </c>
     </row>
     <row r="10">
@@ -1459,7 +1459,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="n">
-        <v>74116.3582598173</v>
+        <v>542344.893745249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>